<commit_message>
Final Commit by Siddhartha
</commit_message>
<xml_diff>
--- a/testData/testexcel.xlsx
+++ b/testData/testexcel.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2303462\eclipse-workspace\GSD_Cognizant\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF122EB-DFA8-4C72-8416-57F399004079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAEACF6-CE34-4315-A307-70384AD908EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{242A8DD4-D49A-4553-8732-62023BAF92E9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{242A8DD4-D49A-4553-8732-62023BAF92E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Lnaguages" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="107">
   <si>
     <t>Languages</t>
   </si>
@@ -367,7 +367,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,7 +383,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,11 +401,6 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -420,24 +414,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,8 +740,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.7265625"/>
-    <col min="2" max="2" customWidth="true" width="10.1796875"/>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
@@ -794,7 +774,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.08984375"/>
+    <col min="1" max="1" width="18.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
@@ -1086,19 +1066,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB9B9B7-2ACB-4586-A066-EB5A3F50EC09}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.36328125"/>
-    <col min="2" max="2" customWidth="true" width="17.6328125"/>
-    <col min="3" max="3" customWidth="true" width="17.26953125"/>
-    <col min="4" max="5" customWidth="true" width="17.36328125"/>
-    <col min="6" max="6" customWidth="true" width="17.453125"/>
-    <col min="7" max="7" customWidth="true" width="17.6328125"/>
-    <col min="8" max="8" customWidth="true" width="17.453125"/>
+    <col min="1" max="1" width="17.36328125" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="5" width="17.36328125" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
@@ -1310,7 +1290,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s" s="14">
+      <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1324,19 +1304,19 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.0"/>
-    <col min="2" max="2" customWidth="true" width="17.7265625"/>
-    <col min="3" max="3" customWidth="true" width="17.6328125"/>
-    <col min="4" max="4" customWidth="true" width="17.81640625"/>
-    <col min="5" max="5" customWidth="true" width="17.36328125"/>
-    <col min="6" max="6" customWidth="true" width="17.453125"/>
-    <col min="7" max="7" customWidth="true" width="17.1796875"/>
-    <col min="8" max="8" customWidth="true" width="18.54296875"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1548,7 +1528,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s" s="15">
+      <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1561,20 +1541,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AEDC4CF-F0FC-4BF6-8FE2-18AB97E2E0FB}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.36328125"/>
-    <col min="2" max="2" customWidth="true" width="17.54296875"/>
-    <col min="3" max="3" customWidth="true" width="17.6328125"/>
-    <col min="4" max="4" customWidth="true" width="17.08984375"/>
-    <col min="5" max="5" customWidth="true" width="17.54296875"/>
-    <col min="6" max="6" customWidth="true" width="16.6328125"/>
-    <col min="7" max="7" customWidth="true" width="17.0"/>
-    <col min="8" max="8" customWidth="true" width="17.81640625"/>
+    <col min="1" max="1" width="17.36328125" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" customWidth="1"/>
+    <col min="4" max="4" width="17.08984375" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" customWidth="1"/>
+    <col min="6" max="6" width="16.6328125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
@@ -1786,7 +1766,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s" s="16">
+      <c r="A11" s="2" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>